<commit_message>
deleted extra testing files
</commit_message>
<xml_diff>
--- a/data/types.xlsx
+++ b/data/types.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="255" windowWidth="18195" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="255" windowWidth="18195" windowHeight="11640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ΜΠΑΛΚΟΝΟΠΟΡΤΕΣ" sheetId="6" r:id="rId1"/>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
@@ -1598,7 +1598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -2914,7 +2914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>